<commit_message>
Updates the IDAN dataset.
Refreshes the IDAN dataset with the latest information.
</commit_message>
<xml_diff>
--- a/idan_data.xlsx
+++ b/idan_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathansheffer/Desktop/College/The Idan research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF63136E-4830-C64A-BA87-43368A071DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F256D9-2989-8849-8BA3-CE2E81195DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{3F58849A-5EA8-AD43-8676-66103A207EE5}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>course</t>
   </si>
@@ -930,10 +930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF495C0-8A69-DA4A-AE6E-47460DC0A5B5}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1074,6 +1074,85 @@
         <v>30</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45798</v>
+      </c>
+      <c r="D7">
+        <v>110</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45798</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4">
+        <v>6.25E-2</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45799</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45799</v>
+      </c>
+      <c r="D10">
+        <v>90</v>
+      </c>
+      <c r="E10" s="4">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
+        <v>45799</v>
+      </c>
+      <c r="D11">
+        <v>120</v>
+      </c>
+      <c r="E11" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="H11">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>